<commit_message>
success add by form and excel
</commit_message>
<xml_diff>
--- a/src/assets/example_file.xlsx
+++ b/src/assets/example_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rawich\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F204C3E-A947-4B95-BDFC-252E1621CE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302879ED-F501-4EA4-A4C3-56F79F6AB403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -90,12 +90,6 @@
     <t>BMS</t>
   </si>
   <si>
-    <t>CRM</t>
-  </si>
-  <si>
-    <t>Backend Developer</t>
-  </si>
-  <si>
     <t>นาย</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>fogus1@gmail.com</t>
   </si>
   <si>
-    <t>Frontend Developer</t>
-  </si>
-  <si>
     <t>นาง</t>
   </si>
   <si>
@@ -162,21 +153,12 @@
     <t>zeeloto@gmail.com</t>
   </si>
   <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>BMs</t>
-  </si>
-  <si>
     <t>มหาวิทยาลัยบูรพา</t>
   </si>
   <si>
     <t>จักร รัตนประเสริฐ</t>
   </si>
   <si>
-    <t>ชลเทพ อรุณรุ่งก้าวไกล</t>
-  </si>
-  <si>
     <t>วิทยาการสารสนเทศ</t>
   </si>
   <si>
@@ -192,24 +174,9 @@
     <t>พนิดา ถำวาปี</t>
   </si>
   <si>
-    <t>กัญญาพร เพ็ชรทอง</t>
-  </si>
-  <si>
-    <t>ธีรจักร สกุลชัยสิทธิโชค</t>
-  </si>
-  <si>
-    <t>Mobile B</t>
-  </si>
-  <si>
     <t>Mobile A</t>
   </si>
   <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Mobile-Dev</t>
-  </si>
-  <si>
     <t>ไอซ์</t>
   </si>
   <si>
@@ -226,6 +193,45 @@
   </si>
   <si>
     <t>วิศวกรรมคอมพิวเตอร์</t>
+  </si>
+  <si>
+    <t>กิตติธร ปรีดาอัครกุล</t>
+  </si>
+  <si>
+    <t>พัฒน์ สุพรรณภาคิน</t>
+  </si>
+  <si>
+    <t>ปริญญา ศิลาดี</t>
+  </si>
+  <si>
+    <t>ปฐมพร ภูพาณิชย์</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Government Project</t>
+  </si>
+  <si>
+    <t>Interactive Media</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Acc Team A</t>
+  </si>
+  <si>
+    <t>BMS Team B</t>
+  </si>
+  <si>
+    <t>BMS Team A</t>
+  </si>
+  <si>
+    <t>Gov Team A</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -256,7 +262,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -270,7 +276,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -318,7 +324,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -701,14 +707,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="28.25" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="19" width="25.7109375" style="5" customWidth="1"/>
-    <col min="20" max="16384" width="28.28515625" style="5"/>
+    <col min="1" max="19" width="25.75" style="5" customWidth="1"/>
+    <col min="20" max="16384" width="28.25" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="22.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -778,28 +782,26 @@
         <v>19</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="J2" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K2" s="11">
         <v>243501</v>
@@ -807,19 +809,19 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="S2" s="6"/>
     </row>
@@ -831,28 +833,26 @@
         <v>19</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>21</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D3" s="15"/>
       <c r="E3" s="9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3" s="11">
         <v>243502</v>
@@ -860,19 +860,19 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="S3" s="9"/>
     </row>
@@ -884,28 +884,28 @@
         <v>19</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K4" s="11">
         <v>243503</v>
@@ -913,19 +913,19 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="Q4" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="S4" s="9"/>
     </row>
@@ -937,28 +937,26 @@
         <v>19</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K5" s="11">
         <v>243504</v>
@@ -966,19 +964,19 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="S5" s="9"/>
     </row>
@@ -990,28 +988,26 @@
         <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K6" s="11">
         <v>243505</v>
@@ -1019,19 +1015,19 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="O6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="R6" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="S6" s="9"/>
     </row>
@@ -1043,46 +1039,46 @@
         <v>19</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="K7" s="11">
         <v>243506</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'fild' of https://github.com/64160271/Team4 into fild"
This reverts commit 639cd865369c12435f9602fac5be8535954edfbd, reversing
changes made to 9a51ad9e6817fde330543c5db172166877c1b4e8.
</commit_message>
<xml_diff>
--- a/src/assets/example_file.xlsx
+++ b/src/assets/example_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rawich\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F204C3E-A947-4B95-BDFC-252E1621CE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302879ED-F501-4EA4-A4C3-56F79F6AB403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -90,12 +90,6 @@
     <t>BMS</t>
   </si>
   <si>
-    <t>CRM</t>
-  </si>
-  <si>
-    <t>Backend Developer</t>
-  </si>
-  <si>
     <t>นาย</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>fogus1@gmail.com</t>
   </si>
   <si>
-    <t>Frontend Developer</t>
-  </si>
-  <si>
     <t>นาง</t>
   </si>
   <si>
@@ -162,21 +153,12 @@
     <t>zeeloto@gmail.com</t>
   </si>
   <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>BMs</t>
-  </si>
-  <si>
     <t>มหาวิทยาลัยบูรพา</t>
   </si>
   <si>
     <t>จักร รัตนประเสริฐ</t>
   </si>
   <si>
-    <t>ชลเทพ อรุณรุ่งก้าวไกล</t>
-  </si>
-  <si>
     <t>วิทยาการสารสนเทศ</t>
   </si>
   <si>
@@ -192,24 +174,9 @@
     <t>พนิดา ถำวาปี</t>
   </si>
   <si>
-    <t>กัญญาพร เพ็ชรทอง</t>
-  </si>
-  <si>
-    <t>ธีรจักร สกุลชัยสิทธิโชค</t>
-  </si>
-  <si>
-    <t>Mobile B</t>
-  </si>
-  <si>
     <t>Mobile A</t>
   </si>
   <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Mobile-Dev</t>
-  </si>
-  <si>
     <t>ไอซ์</t>
   </si>
   <si>
@@ -226,6 +193,45 @@
   </si>
   <si>
     <t>วิศวกรรมคอมพิวเตอร์</t>
+  </si>
+  <si>
+    <t>กิตติธร ปรีดาอัครกุล</t>
+  </si>
+  <si>
+    <t>พัฒน์ สุพรรณภาคิน</t>
+  </si>
+  <si>
+    <t>ปริญญา ศิลาดี</t>
+  </si>
+  <si>
+    <t>ปฐมพร ภูพาณิชย์</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Government Project</t>
+  </si>
+  <si>
+    <t>Interactive Media</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Acc Team A</t>
+  </si>
+  <si>
+    <t>BMS Team B</t>
+  </si>
+  <si>
+    <t>BMS Team A</t>
+  </si>
+  <si>
+    <t>Gov Team A</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -256,7 +262,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -270,7 +276,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -318,7 +324,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -701,14 +707,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="28.25" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="19" width="25.7109375" style="5" customWidth="1"/>
-    <col min="20" max="16384" width="28.28515625" style="5"/>
+    <col min="1" max="19" width="25.75" style="5" customWidth="1"/>
+    <col min="20" max="16384" width="28.25" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="22.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -778,28 +782,26 @@
         <v>19</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D2" s="8"/>
       <c r="E2" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="J2" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K2" s="11">
         <v>243501</v>
@@ -807,19 +809,19 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="S2" s="6"/>
     </row>
@@ -831,28 +833,26 @@
         <v>19</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>21</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D3" s="15"/>
       <c r="E3" s="9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3" s="11">
         <v>243502</v>
@@ -860,19 +860,19 @@
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="S3" s="9"/>
     </row>
@@ -884,28 +884,28 @@
         <v>19</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K4" s="11">
         <v>243503</v>
@@ -913,19 +913,19 @@
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="Q4" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="S4" s="9"/>
     </row>
@@ -937,28 +937,26 @@
         <v>19</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K5" s="11">
         <v>243504</v>
@@ -966,19 +964,19 @@
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="S5" s="9"/>
     </row>
@@ -990,28 +988,26 @@
         <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K6" s="11">
         <v>243505</v>
@@ -1019,19 +1015,19 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="O6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="R6" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="S6" s="9"/>
     </row>
@@ -1043,46 +1039,46 @@
         <v>19</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="K7" s="11">
         <v>243506</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>